<commit_message>
PM angepasst und ins Dokument eingefügt
</commit_message>
<xml_diff>
--- a/Planung/03_Design/Projektmanagement_Design.xlsx
+++ b/Planung/03_Design/Projektmanagement_Design.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>Projektmanagement</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Zusammenfassung</t>
+  </si>
+  <si>
+    <t>SS / FB</t>
+  </si>
+  <si>
+    <t>alle</t>
   </si>
 </sst>
 </file>
@@ -255,7 +261,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -263,6 +269,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,13 +292,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
@@ -296,6 +308,8 @@
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Schlecht" xfId="6" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -676,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1063,7 +1077,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>25</v>
@@ -1077,7 +1091,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>26</v>
@@ -1091,7 +1105,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>27</v>
@@ -1133,7 +1147,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>23</v>

</xml_diff>